<commit_message>
KIBON-120: Mitarbeiterinnen statistic translated
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Mitarbeiterinnen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Mitarbeiterinnen.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\C$\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA13428-F6DB-4F44-B30D-0A78DEAB02C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,27 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Mitarbeiterinnen Jugendamt</t>
-  </si>
-  <si>
-    <t>Von</t>
-  </si>
-  <si>
-    <t>Bis</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Anzahl verantwortliche Gesuche</t>
-  </si>
-  <si>
-    <t>Verfügungen ausgestellt</t>
-  </si>
-  <si>
     <t>{auswertungVon}</t>
   </si>
   <si>
@@ -66,12 +46,33 @@
   </si>
   <si>
     <t>{repeatMitarbeiterinnenRow}</t>
+  </si>
+  <si>
+    <t>{nachnameTitle}</t>
+  </si>
+  <si>
+    <t>{vornameTitle}</t>
+  </si>
+  <si>
+    <t>{anzahlVerGesucheTitle}</t>
+  </si>
+  <si>
+    <t>{verfuegungAusgestelltTitle}</t>
+  </si>
+  <si>
+    <t>{vonTitle}</t>
+  </si>
+  <si>
+    <t>{bisTitle}</t>
+  </si>
+  <si>
+    <t>{mitarbeiterinnenTitle}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -464,11 +465,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +482,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -491,19 +492,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="7"/>
@@ -513,33 +514,33 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
KIBON-120: corrupt statistic Benutzer and Mitarbeiter fixed
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Mitarbeiterinnen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Mitarbeiterinnen.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\reporting_new\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reporting_new\new\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968423A1-FADE-4B4C-8A83-4FC45FD76AEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13965" xr2:uid="{58351B0B-949B-4D11-ABB2-DE489F1554AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -26,12 +33,33 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
+    <t>{mitarbeiterinnenTitle}</t>
+  </si>
+  <si>
+    <t>{vonTitle}</t>
+  </si>
+  <si>
+    <t>{bisTitle}</t>
+  </si>
+  <si>
     <t>{auswertungVon}</t>
   </si>
   <si>
     <t>{auswertungBis}</t>
   </si>
   <si>
+    <t>{nachnameTitle}</t>
+  </si>
+  <si>
+    <t>{vornameTitle}</t>
+  </si>
+  <si>
+    <t>{anzahlVerGesucheTitle}</t>
+  </si>
+  <si>
+    <t>{verfuegungAusgestelltTitle}</t>
+  </si>
+  <si>
     <t>{name}</t>
   </si>
   <si>
@@ -45,43 +73,14 @@
   </si>
   <si>
     <t>{repeatMitarbeiterinnenRow}</t>
-  </si>
-  <si>
-    <t>{nachnameTitle}</t>
-  </si>
-  <si>
-    <t>{vornameTitle}</t>
-  </si>
-  <si>
-    <t>{anzahlVerGesucheTitle}</t>
-  </si>
-  <si>
-    <t>{verfuegungAusgestelltTitle}</t>
-  </si>
-  <si>
-    <t>{vonTitle}</t>
-  </si>
-  <si>
-    <t>{bisTitle}</t>
-  </si>
-  <si>
-    <t>{mitarbeiterinnenTitle}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -117,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,51 +139,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -203,7 +173,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -219,7 +189,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -231,7 +201,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -248,9 +218,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -278,14 +248,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -313,6 +300,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -464,114 +468,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27793105-0DD8-4954-A1B4-5AC5B3F2028C}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>